<commit_message>
Move all renewables to guaranteed dispatch and out of least cost dispatch with new logit dispatch function
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96458CF2-F2C8-4081-BA0C-8387800D0428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BGDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,6 +255,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -278,6 +307,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,10 +499,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -512,13 +560,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1236,147 +1286,147 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -1384,147 +1434,147 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -1532,147 +1582,147 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -2420,147 +2470,147 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>$B14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated EDLE to closely align with 2020 generation and BGDPbES to move all non dispatchable resources to guaranteed dispatch (geothermal, biomass, MSW, all other renewables).
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96458CF2-F2C8-4081-BA0C-8387800D0428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257288C8-88AB-4482-B0B3-D67DC1B2D04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,147 +1730,147 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
         <f t="shared" ref="D9:AK14" si="2">$B9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -1878,147 +1878,147 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -2844,112 +2844,147 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <f>B17</f>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <f t="shared" ref="D17:AK17" si="3">C17</f>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Y17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Z17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AB17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AC17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AD17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AE17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AF17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AG17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AH17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AI17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AJ17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AK17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2020 guaranteed dispatch setting for coal
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE88CF1-B83D-4142-BD38-2B2172C8BD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73A0787-3581-4D21-A9CD-91111CFCA519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="351">
   <si>
     <t>Notes:</t>
   </si>
@@ -1086,6 +1086,9 @@
   </si>
   <si>
     <t>Difference</t>
+  </si>
+  <si>
+    <t>Calibration multiplier (used to ensure 2020 output in the model aligns with STEO)</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1140,6 +1143,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1481,7 +1487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1575,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB677FF-8AA7-4A99-AA5C-83E52BC9397F}">
   <dimension ref="A1:BB120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8096,85 +8102,85 @@
         <v>188.452</v>
       </c>
       <c r="F2">
-        <v>181.614</v>
+        <v>180.82499999999999</v>
       </c>
       <c r="G2">
-        <v>161.88900000000001</v>
+        <v>157.94399999999999</v>
       </c>
       <c r="H2">
-        <v>155.05099999999999</v>
+        <v>149.00200000000001</v>
       </c>
       <c r="I2">
-        <v>148.739</v>
+        <v>141.11199999999999</v>
       </c>
       <c r="J2">
-        <v>137.69300000000001</v>
+        <v>128.22499999999999</v>
       </c>
       <c r="K2">
-        <v>126.64700000000001</v>
+        <v>120.598</v>
       </c>
       <c r="L2">
-        <v>121.913</v>
+        <v>115.864</v>
       </c>
       <c r="M2">
-        <v>121.387</v>
+        <v>115.33799999999999</v>
       </c>
       <c r="N2">
-        <v>119.02</v>
+        <v>112.971</v>
       </c>
       <c r="O2">
-        <v>118.494</v>
+        <v>112.708</v>
       </c>
       <c r="P2">
-        <v>113.497</v>
+        <v>108.76300000000001</v>
       </c>
       <c r="Q2">
-        <v>111.919</v>
+        <v>107.44799999999999</v>
       </c>
       <c r="R2">
-        <v>111.13</v>
+        <v>107.185</v>
       </c>
       <c r="S2">
-        <v>110.867</v>
+        <v>107.185</v>
       </c>
       <c r="T2">
-        <v>109.815</v>
+        <v>106.133</v>
       </c>
       <c r="U2">
-        <v>109.815</v>
+        <v>106.133</v>
       </c>
       <c r="V2">
-        <v>108.23699999999999</v>
+        <v>104.55500000000001</v>
       </c>
       <c r="W2">
-        <v>108.23699999999999</v>
+        <v>104.55500000000001</v>
       </c>
       <c r="X2">
-        <v>108.23699999999999</v>
+        <v>104.55500000000001</v>
       </c>
       <c r="Y2">
-        <v>108.23699999999999</v>
+        <v>104.55500000000001</v>
       </c>
       <c r="Z2">
-        <v>108.23699999999999</v>
+        <v>104.55500000000001</v>
       </c>
       <c r="AA2">
-        <v>105.87</v>
+        <v>102.188</v>
       </c>
       <c r="AB2">
-        <v>105.87</v>
+        <v>102.188</v>
       </c>
       <c r="AC2">
-        <v>105.87</v>
+        <v>102.188</v>
       </c>
       <c r="AD2">
-        <v>105.87</v>
+        <v>102.188</v>
       </c>
       <c r="AE2">
-        <v>105.87</v>
+        <v>102.188</v>
       </c>
       <c r="AF2">
-        <v>105.87</v>
+        <v>102.188</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
@@ -8191,88 +8197,88 @@
         <v>345.38200000000001</v>
       </c>
       <c r="E3">
-        <v>342.57400000000001</v>
+        <v>343.19799999999998</v>
       </c>
       <c r="F3">
-        <v>336.178</v>
+        <v>336.334</v>
       </c>
       <c r="G3">
-        <v>337.11399999999998</v>
+        <v>336.49</v>
       </c>
       <c r="H3">
-        <v>334.93</v>
+        <v>333.37</v>
       </c>
       <c r="I3">
-        <v>334.15</v>
+        <v>332.12200000000001</v>
       </c>
       <c r="J3">
-        <v>334.61799999999999</v>
+        <v>332.74599999999998</v>
       </c>
       <c r="K3">
-        <v>334.30599999999998</v>
+        <v>331.96600000000001</v>
       </c>
       <c r="L3">
-        <v>334.46199999999999</v>
+        <v>330.87400000000002</v>
       </c>
       <c r="M3">
-        <v>333.99400000000003</v>
+        <v>330.25</v>
       </c>
       <c r="N3">
-        <v>333.83800000000002</v>
+        <v>330.56200000000001</v>
       </c>
       <c r="O3">
-        <v>333.68200000000002</v>
+        <v>330.25</v>
       </c>
       <c r="P3">
-        <v>333.83800000000002</v>
+        <v>330.09399999999999</v>
       </c>
       <c r="Q3">
-        <v>332.59</v>
+        <v>329.62599999999998</v>
       </c>
       <c r="R3">
-        <v>332.27800000000002</v>
+        <v>329.15800000000002</v>
       </c>
       <c r="S3">
-        <v>331.654</v>
+        <v>329.47</v>
       </c>
       <c r="T3">
-        <v>331.96600000000001</v>
+        <v>329.78199999999998</v>
       </c>
       <c r="U3">
-        <v>332.27800000000002</v>
+        <v>330.09399999999999</v>
       </c>
       <c r="V3">
-        <v>332.12200000000001</v>
+        <v>329.78199999999998</v>
       </c>
       <c r="W3">
-        <v>332.43400000000003</v>
+        <v>329.93799999999999</v>
       </c>
       <c r="X3">
-        <v>332.27800000000002</v>
+        <v>329.78199999999998</v>
       </c>
       <c r="Y3">
-        <v>332.43400000000003</v>
+        <v>329.93799999999999</v>
       </c>
       <c r="Z3">
-        <v>331.96600000000001</v>
+        <v>330.09399999999999</v>
       </c>
       <c r="AA3">
-        <v>332.27800000000002</v>
+        <v>330.25</v>
       </c>
       <c r="AB3">
-        <v>332.43400000000003</v>
+        <v>330.40600000000001</v>
       </c>
       <c r="AC3">
-        <v>332.59</v>
+        <v>330.56200000000001</v>
       </c>
       <c r="AD3">
-        <v>332.74599999999998</v>
+        <v>330.71800000000002</v>
       </c>
       <c r="AE3">
-        <v>331.654</v>
+        <v>330.87400000000002</v>
       </c>
       <c r="AF3">
-        <v>331.654</v>
+        <v>331.03</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -8304,73 +8310,73 @@
         <v>93.619</v>
       </c>
       <c r="J4">
-        <v>88.619</v>
+        <v>86.619</v>
       </c>
       <c r="K4">
-        <v>87.619</v>
+        <v>85.619</v>
       </c>
       <c r="L4">
-        <v>86.619</v>
+        <v>85.619</v>
       </c>
       <c r="M4">
-        <v>86.619</v>
+        <v>85.619</v>
       </c>
       <c r="N4">
-        <v>86.619</v>
+        <v>85.619</v>
       </c>
       <c r="O4">
-        <v>81.619</v>
+        <v>79.619</v>
       </c>
       <c r="P4">
-        <v>81.619</v>
+        <v>79.619</v>
       </c>
       <c r="Q4">
-        <v>81.619</v>
+        <v>78.619</v>
       </c>
       <c r="R4">
-        <v>81.619</v>
+        <v>78.619</v>
       </c>
       <c r="S4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="T4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="U4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="V4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="W4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="X4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="Y4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="Z4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="AA4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="AB4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="AC4">
-        <v>80.619</v>
+        <v>78.619</v>
       </c>
       <c r="AD4">
-        <v>79.619</v>
+        <v>78.619</v>
       </c>
       <c r="AE4">
-        <v>79.619</v>
+        <v>78.619</v>
       </c>
       <c r="AF4">
-        <v>79.619</v>
+        <v>78.619</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
@@ -8393,82 +8399,82 @@
         <v>79.891000000000005</v>
       </c>
       <c r="G5">
-        <v>79.828000000000003</v>
+        <v>79.820999999999998</v>
       </c>
       <c r="H5">
-        <v>79.778000000000006</v>
+        <v>79.772999999999996</v>
       </c>
       <c r="I5">
-        <v>79.724999999999994</v>
+        <v>79.703000000000003</v>
       </c>
       <c r="J5">
-        <v>79.438000000000002</v>
+        <v>79.429000000000002</v>
       </c>
       <c r="K5">
-        <v>79.298000000000002</v>
+        <v>79.275999999999996</v>
       </c>
       <c r="L5">
-        <v>79.28</v>
+        <v>79.188000000000002</v>
       </c>
       <c r="M5">
-        <v>79.269000000000005</v>
+        <v>79.188000000000002</v>
       </c>
       <c r="N5">
-        <v>79.269000000000005</v>
+        <v>79.188000000000002</v>
       </c>
       <c r="O5">
-        <v>79.225999999999999</v>
+        <v>79.188000000000002</v>
       </c>
       <c r="P5">
-        <v>79.188000000000002</v>
+        <v>79.173000000000002</v>
       </c>
       <c r="Q5">
-        <v>79.188000000000002</v>
+        <v>79.173000000000002</v>
       </c>
       <c r="R5">
-        <v>79.188000000000002</v>
+        <v>79.173000000000002</v>
       </c>
       <c r="S5">
-        <v>79.188000000000002</v>
+        <v>79.171999999999997</v>
       </c>
       <c r="T5">
-        <v>79.188000000000002</v>
+        <v>79.171999999999997</v>
       </c>
       <c r="U5">
-        <v>79.188000000000002</v>
+        <v>79.162000000000006</v>
       </c>
       <c r="V5">
-        <v>79.188000000000002</v>
+        <v>79.162000000000006</v>
       </c>
       <c r="W5">
-        <v>79.188000000000002</v>
+        <v>79.162000000000006</v>
       </c>
       <c r="X5">
-        <v>79.188000000000002</v>
+        <v>79.162000000000006</v>
       </c>
       <c r="Y5">
-        <v>79.188000000000002</v>
+        <v>79.162000000000006</v>
       </c>
       <c r="Z5">
-        <v>79.096000000000004</v>
+        <v>79.081999999999994</v>
       </c>
       <c r="AA5">
-        <v>79.046000000000006</v>
+        <v>79.081999999999994</v>
       </c>
       <c r="AB5">
-        <v>79.043999999999997</v>
+        <v>79.08</v>
       </c>
       <c r="AC5">
-        <v>79.040999999999997</v>
+        <v>79.076999999999998</v>
       </c>
       <c r="AD5">
-        <v>79.040999999999997</v>
+        <v>79.076999999999998</v>
       </c>
       <c r="AE5">
-        <v>79.025999999999996</v>
+        <v>79.06</v>
       </c>
       <c r="AF5">
-        <v>79.024000000000001</v>
+        <v>78.998999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
@@ -8488,85 +8494,85 @@
         <v>145.48400000000001</v>
       </c>
       <c r="F6">
-        <v>148.864</v>
+        <v>147.82900000000001</v>
       </c>
       <c r="G6">
-        <v>164.084</v>
+        <v>156.10400000000001</v>
       </c>
       <c r="H6">
-        <v>176.21899999999999</v>
+        <v>167.089</v>
       </c>
       <c r="I6">
-        <v>186.42400000000001</v>
+        <v>176.07400000000001</v>
       </c>
       <c r="J6">
-        <v>202.29900000000001</v>
+        <v>193.53399999999999</v>
       </c>
       <c r="K6">
-        <v>214.184</v>
+        <v>202.239</v>
       </c>
       <c r="L6">
-        <v>222.00899999999999</v>
+        <v>208.149</v>
       </c>
       <c r="M6">
-        <v>227.84899999999999</v>
+        <v>212.54400000000001</v>
       </c>
       <c r="N6">
-        <v>235.149</v>
+        <v>218.834</v>
       </c>
       <c r="O6">
-        <v>246.274</v>
+        <v>229.934</v>
       </c>
       <c r="P6">
-        <v>254.96899999999999</v>
+        <v>236.79400000000001</v>
       </c>
       <c r="Q6">
-        <v>262.959</v>
+        <v>243.92400000000001</v>
       </c>
       <c r="R6">
-        <v>270.18400000000003</v>
+        <v>249.809</v>
       </c>
       <c r="S6">
-        <v>278.47899999999998</v>
+        <v>255.524</v>
       </c>
       <c r="T6">
-        <v>285.76900000000001</v>
+        <v>261.25400000000002</v>
       </c>
       <c r="U6">
-        <v>292.13900000000001</v>
+        <v>266.49900000000002</v>
       </c>
       <c r="V6">
-        <v>298.73899999999998</v>
+        <v>271.70400000000001</v>
       </c>
       <c r="W6">
-        <v>305.28399999999999</v>
+        <v>276.81400000000002</v>
       </c>
       <c r="X6">
-        <v>311.714</v>
+        <v>281.85899999999998</v>
       </c>
       <c r="Y6">
-        <v>318.11399999999998</v>
+        <v>286.93900000000002</v>
       </c>
       <c r="Z6">
-        <v>324.36399999999998</v>
+        <v>291.73399999999998</v>
       </c>
       <c r="AA6">
-        <v>331.97399999999999</v>
+        <v>297.84899999999999</v>
       </c>
       <c r="AB6">
-        <v>338.19400000000002</v>
+        <v>303.44900000000001</v>
       </c>
       <c r="AC6">
-        <v>344.48399999999998</v>
+        <v>308.88900000000001</v>
       </c>
       <c r="AD6">
-        <v>351.13400000000001</v>
+        <v>313.899</v>
       </c>
       <c r="AE6">
-        <v>357.92399999999998</v>
+        <v>319.30399999999997</v>
       </c>
       <c r="AF6">
-        <v>364.99400000000003</v>
+        <v>325.39400000000001</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -8586,85 +8592,85 @@
         <v>100.98699999999999</v>
       </c>
       <c r="F7">
-        <v>107.04900000000001</v>
+        <v>106.083</v>
       </c>
       <c r="G7">
-        <v>127.80500000000001</v>
+        <v>116.15900000000001</v>
       </c>
       <c r="H7">
-        <v>141.64099999999999</v>
+        <v>128.58699999999999</v>
       </c>
       <c r="I7">
-        <v>155.20500000000001</v>
+        <v>140.51499999999999</v>
       </c>
       <c r="J7">
-        <v>178.441</v>
+        <v>166.035</v>
       </c>
       <c r="K7">
-        <v>197.291</v>
+        <v>179.857</v>
       </c>
       <c r="L7">
-        <v>211.11500000000001</v>
+        <v>190.309</v>
       </c>
       <c r="M7">
-        <v>221.66300000000001</v>
+        <v>198.26900000000001</v>
       </c>
       <c r="N7">
-        <v>235.23500000000001</v>
+        <v>209.995</v>
       </c>
       <c r="O7">
-        <v>256.267</v>
+        <v>231.059</v>
       </c>
       <c r="P7">
-        <v>272.89699999999999</v>
+        <v>244.25899999999999</v>
       </c>
       <c r="Q7">
-        <v>288.36500000000001</v>
+        <v>258.15699999999998</v>
       </c>
       <c r="R7">
-        <v>302.62700000000001</v>
+        <v>269.86099999999999</v>
       </c>
       <c r="S7">
-        <v>319.14499999999998</v>
+        <v>281.35500000000002</v>
       </c>
       <c r="T7">
-        <v>333.767</v>
+        <v>292.97699999999998</v>
       </c>
       <c r="U7">
-        <v>346.63299999999998</v>
+        <v>303.70100000000002</v>
       </c>
       <c r="V7">
-        <v>360.15300000000002</v>
+        <v>314.50900000000001</v>
       </c>
       <c r="W7">
-        <v>373.61700000000002</v>
+        <v>325.19299999999998</v>
       </c>
       <c r="X7">
-        <v>386.887</v>
+        <v>335.791</v>
       </c>
       <c r="Y7">
-        <v>400.13900000000001</v>
+        <v>346.50900000000001</v>
       </c>
       <c r="Z7">
-        <v>413.21499999999997</v>
+        <v>356.74299999999999</v>
       </c>
       <c r="AA7">
-        <v>429.14100000000002</v>
+        <v>369.81299999999999</v>
       </c>
       <c r="AB7">
-        <v>442.15699999999998</v>
+        <v>381.803</v>
       </c>
       <c r="AC7">
-        <v>455.303</v>
+        <v>393.45299999999997</v>
       </c>
       <c r="AD7">
-        <v>469.30900000000003</v>
+        <v>404.27499999999998</v>
       </c>
       <c r="AE7">
-        <v>483.58100000000002</v>
+        <v>415.95499999999998</v>
       </c>
       <c r="AF7">
-        <v>498.40899999999999</v>
+        <v>429.08699999999999</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.35">
@@ -8687,82 +8693,82 @@
         <v>1.758</v>
       </c>
       <c r="G8">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="H8">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="I8">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="J8">
         <v>2.0699999999999998</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>2.0699999999999998</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>2.0699999999999998</v>
       </c>
-      <c r="J8">
-        <v>2.226</v>
-      </c>
-      <c r="K8">
-        <v>2.226</v>
-      </c>
-      <c r="L8">
-        <v>2.226</v>
-      </c>
       <c r="M8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="N8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="O8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="P8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="R8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="S8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="T8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="U8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="V8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="W8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="X8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Y8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Z8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="AA8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="AB8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="AC8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="AD8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="AE8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="AF8">
-        <v>2.226</v>
+        <v>2.0699999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.35">
@@ -8785,82 +8791,82 @@
         <v>4.9969999999999999</v>
       </c>
       <c r="G9">
+        <v>5.0149999999999997</v>
+      </c>
+      <c r="H9">
         <v>5.0330000000000004</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>5.0510000000000002</v>
-      </c>
-      <c r="I9">
-        <v>5.069</v>
       </c>
       <c r="J9">
         <v>5.0869999999999997</v>
       </c>
       <c r="K9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="L9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="M9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="N9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="O9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="P9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="Q9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="R9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="S9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="T9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="U9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="V9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="W9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="X9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="Y9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="Z9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="AA9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="AB9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="AC9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="AD9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="AE9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
       <c r="AF9">
-        <v>5.1050000000000004</v>
+        <v>5.0869999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
@@ -8883,82 +8889,82 @@
         <v>2.597</v>
       </c>
       <c r="G10">
-        <v>2.714</v>
+        <v>2.649</v>
       </c>
       <c r="H10">
-        <v>2.8050000000000002</v>
+        <v>2.7269999999999999</v>
       </c>
       <c r="I10">
-        <v>2.883</v>
+        <v>2.7919999999999998</v>
       </c>
       <c r="J10">
+        <v>2.9220000000000002</v>
+      </c>
+      <c r="K10">
+        <v>2.9740000000000002</v>
+      </c>
+      <c r="L10">
         <v>3</v>
       </c>
-      <c r="K10">
-        <v>3.0779999999999998</v>
-      </c>
-      <c r="L10">
+      <c r="M10">
+        <v>3.0259999999999998</v>
+      </c>
+      <c r="N10">
+        <v>3.052</v>
+      </c>
+      <c r="O10">
         <v>3.117</v>
       </c>
-      <c r="M10">
+      <c r="P10">
         <v>3.1429999999999998</v>
       </c>
-      <c r="N10">
-        <v>3.1819999999999999</v>
-      </c>
-      <c r="O10">
-        <v>3.234</v>
-      </c>
-      <c r="P10">
+      <c r="Q10">
+        <v>3.169</v>
+      </c>
+      <c r="R10">
+        <v>3.1949999999999998</v>
+      </c>
+      <c r="S10">
+        <v>3.2210000000000001</v>
+      </c>
+      <c r="T10">
+        <v>3.2469999999999999</v>
+      </c>
+      <c r="U10">
+        <v>3.26</v>
+      </c>
+      <c r="V10">
         <v>3.2730000000000001</v>
       </c>
-      <c r="Q10">
+      <c r="W10">
+        <v>3.286</v>
+      </c>
+      <c r="X10">
+        <v>3.2989999999999999</v>
+      </c>
+      <c r="Y10">
         <v>3.3119999999999998</v>
       </c>
-      <c r="R10">
+      <c r="Z10">
+        <v>3.3250000000000002</v>
+      </c>
+      <c r="AA10">
         <v>3.3380000000000001</v>
       </c>
-      <c r="S10">
+      <c r="AB10">
+        <v>3.351</v>
+      </c>
+      <c r="AC10">
+        <v>3.3639999999999999</v>
+      </c>
+      <c r="AD10">
         <v>3.3769999999999998</v>
       </c>
-      <c r="T10">
+      <c r="AE10">
+        <v>3.39</v>
+      </c>
+      <c r="AF10">
         <v>3.403</v>
-      </c>
-      <c r="U10">
-        <v>3.4289999999999998</v>
-      </c>
-      <c r="V10">
-        <v>3.4550000000000001</v>
-      </c>
-      <c r="W10">
-        <v>3.4809999999999999</v>
-      </c>
-      <c r="X10">
-        <v>3.5070000000000001</v>
-      </c>
-      <c r="Y10">
-        <v>3.5329999999999999</v>
-      </c>
-      <c r="Z10">
-        <v>3.5459999999999998</v>
-      </c>
-      <c r="AA10">
-        <v>3.5720000000000001</v>
-      </c>
-      <c r="AB10">
-        <v>3.585</v>
-      </c>
-      <c r="AC10">
-        <v>3.5979999999999999</v>
-      </c>
-      <c r="AD10">
-        <v>3.6110000000000002</v>
-      </c>
-      <c r="AE10">
-        <v>3.6240000000000001</v>
-      </c>
-      <c r="AF10">
-        <v>3.637</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.35">
@@ -8984,79 +8990,79 @@
         <v>26.425000000000001</v>
       </c>
       <c r="H11">
-        <v>26.436</v>
+        <v>26.442</v>
       </c>
       <c r="I11">
-        <v>26.456</v>
+        <v>26.466000000000001</v>
       </c>
       <c r="J11">
-        <v>26.478999999999999</v>
+        <v>26.49</v>
       </c>
       <c r="K11">
-        <v>26.501000000000001</v>
+        <v>26.509</v>
       </c>
       <c r="L11">
-        <v>26.515000000000001</v>
+        <v>26.524000000000001</v>
       </c>
       <c r="M11">
-        <v>26.527000000000001</v>
+        <v>26.536999999999999</v>
       </c>
       <c r="N11">
-        <v>26.54</v>
+        <v>26.55</v>
       </c>
       <c r="O11">
-        <v>26.547999999999998</v>
+        <v>26.556999999999999</v>
       </c>
       <c r="P11">
-        <v>26.56</v>
+        <v>26.568999999999999</v>
       </c>
       <c r="Q11">
-        <v>26.571999999999999</v>
+        <v>26.579000000000001</v>
       </c>
       <c r="R11">
-        <v>26.584</v>
+        <v>26.591000000000001</v>
       </c>
       <c r="S11">
-        <v>26.594000000000001</v>
+        <v>26.6</v>
       </c>
       <c r="T11">
-        <v>26.603999999999999</v>
+        <v>26.61</v>
       </c>
       <c r="U11">
-        <v>26.613</v>
+        <v>26.62</v>
       </c>
       <c r="V11">
-        <v>26.623000000000001</v>
+        <v>26.63</v>
       </c>
       <c r="W11">
-        <v>26.632000000000001</v>
+        <v>26.638999999999999</v>
       </c>
       <c r="X11">
-        <v>26.640999999999998</v>
+        <v>26.648</v>
       </c>
       <c r="Y11">
-        <v>26.649000000000001</v>
+        <v>26.655999999999999</v>
       </c>
       <c r="Z11">
-        <v>26.658000000000001</v>
+        <v>26.664000000000001</v>
       </c>
       <c r="AA11">
-        <v>26.667000000000002</v>
+        <v>26.672999999999998</v>
       </c>
       <c r="AB11">
-        <v>26.675000000000001</v>
+        <v>26.681000000000001</v>
       </c>
       <c r="AC11">
-        <v>26.683</v>
+        <v>26.689</v>
       </c>
       <c r="AD11">
-        <v>26.690999999999999</v>
+        <v>26.698</v>
       </c>
       <c r="AE11">
-        <v>26.7</v>
+        <v>26.706</v>
       </c>
       <c r="AF11">
-        <v>26.709</v>
+        <v>26.716000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
@@ -9079,82 +9085,82 @@
         <v>133.59899999999999</v>
       </c>
       <c r="G12">
-        <v>133.649</v>
+        <v>133.54900000000001</v>
       </c>
       <c r="H12">
-        <v>138.59899999999999</v>
+        <v>140.999</v>
       </c>
       <c r="I12">
-        <v>146.69900000000001</v>
+        <v>150.54900000000001</v>
       </c>
       <c r="J12">
-        <v>155.44900000000001</v>
+        <v>159.399</v>
       </c>
       <c r="K12">
-        <v>165.649</v>
+        <v>168.249</v>
       </c>
       <c r="L12">
-        <v>173.59899999999999</v>
+        <v>176.54900000000001</v>
       </c>
       <c r="M12">
-        <v>180.649</v>
+        <v>183.399</v>
       </c>
       <c r="N12">
-        <v>187.649</v>
+        <v>189.69900000000001</v>
       </c>
       <c r="O12">
-        <v>192.19900000000001</v>
+        <v>193.499</v>
       </c>
       <c r="P12">
-        <v>199.249</v>
+        <v>199.999</v>
       </c>
       <c r="Q12">
-        <v>206.499</v>
+        <v>205.94900000000001</v>
       </c>
       <c r="R12">
-        <v>213.399</v>
+        <v>212.44900000000001</v>
       </c>
       <c r="S12">
-        <v>220.29900000000001</v>
+        <v>218.399</v>
       </c>
       <c r="T12">
-        <v>227.34899999999999</v>
+        <v>224.899</v>
       </c>
       <c r="U12">
-        <v>233.84899999999999</v>
+        <v>230.999</v>
       </c>
       <c r="V12">
-        <v>240.79900000000001</v>
+        <v>237.59899999999999</v>
       </c>
       <c r="W12">
-        <v>246.899</v>
+        <v>242.999</v>
       </c>
       <c r="X12">
-        <v>253.399</v>
+        <v>249.149</v>
       </c>
       <c r="Y12">
-        <v>259.899</v>
+        <v>255.249</v>
       </c>
       <c r="Z12">
-        <v>267.44900000000001</v>
+        <v>261.79899999999998</v>
       </c>
       <c r="AA12">
-        <v>275.09899999999999</v>
+        <v>268.649</v>
       </c>
       <c r="AB12">
-        <v>282.44900000000001</v>
+        <v>275.649</v>
       </c>
       <c r="AC12">
-        <v>290.149</v>
+        <v>282.99900000000002</v>
       </c>
       <c r="AD12">
-        <v>297.399</v>
+        <v>290.34899999999999</v>
       </c>
       <c r="AE12">
+        <v>297.59899999999999</v>
+      </c>
+      <c r="AF12">
         <v>305.649</v>
-      </c>
-      <c r="AF12">
-        <v>314.34899999999999</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
@@ -9272,85 +9278,85 @@
         <v>3.9E-2</v>
       </c>
       <c r="F14">
-        <v>1.9790000000000001</v>
+        <v>1.9590000000000001</v>
       </c>
       <c r="G14">
-        <v>2.4889999999999999</v>
+        <v>2.194</v>
       </c>
       <c r="H14">
-        <v>3.0339999999999998</v>
+        <v>2.6890000000000001</v>
       </c>
       <c r="I14">
-        <v>4.7089999999999996</v>
+        <v>4.3040000000000003</v>
       </c>
       <c r="J14">
-        <v>5.3739999999999997</v>
+        <v>5.0190000000000001</v>
       </c>
       <c r="K14">
-        <v>5.6189999999999998</v>
+        <v>5.194</v>
       </c>
       <c r="L14">
-        <v>5.7690000000000001</v>
+        <v>5.3090000000000002</v>
       </c>
       <c r="M14">
-        <v>5.8840000000000003</v>
+        <v>5.3940000000000001</v>
       </c>
       <c r="N14">
-        <v>6.0339999999999998</v>
+        <v>5.5190000000000001</v>
       </c>
       <c r="O14">
-        <v>6.2690000000000001</v>
+        <v>5.7489999999999997</v>
       </c>
       <c r="P14">
-        <v>6.4539999999999997</v>
+        <v>5.8940000000000001</v>
       </c>
       <c r="Q14">
-        <v>6.6239999999999997</v>
+        <v>6.0439999999999996</v>
       </c>
       <c r="R14">
-        <v>6.7839999999999998</v>
+        <v>6.1740000000000004</v>
       </c>
       <c r="S14">
-        <v>6.9690000000000003</v>
+        <v>6.2990000000000004</v>
       </c>
       <c r="T14">
-        <v>7.1340000000000003</v>
+        <v>6.4290000000000003</v>
       </c>
       <c r="U14">
-        <v>7.2789999999999999</v>
+        <v>6.5490000000000004</v>
       </c>
       <c r="V14">
-        <v>7.4340000000000002</v>
+        <v>6.6689999999999996</v>
       </c>
       <c r="W14">
-        <v>7.5890000000000004</v>
+        <v>6.7889999999999997</v>
       </c>
       <c r="X14">
-        <v>7.7439999999999998</v>
+        <v>6.9089999999999998</v>
       </c>
       <c r="Y14">
-        <v>7.9039999999999999</v>
+        <v>7.0339999999999998</v>
       </c>
       <c r="Z14">
-        <v>8.0589999999999993</v>
+        <v>7.1539999999999999</v>
       </c>
       <c r="AA14">
-        <v>8.2490000000000006</v>
+        <v>7.3090000000000002</v>
       </c>
       <c r="AB14">
-        <v>8.4090000000000007</v>
+        <v>7.4539999999999997</v>
       </c>
       <c r="AC14">
-        <v>8.5690000000000008</v>
+        <v>7.5940000000000003</v>
       </c>
       <c r="AD14">
-        <v>8.7439999999999998</v>
+        <v>7.7240000000000002</v>
       </c>
       <c r="AE14">
-        <v>8.9239999999999995</v>
+        <v>7.8639999999999999</v>
       </c>
       <c r="AF14">
-        <v>9.109</v>
+        <v>8.0239999999999991</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.35">
@@ -9581,70 +9587,70 @@
         <v>1.92</v>
       </c>
       <c r="K17">
+        <v>1.9359999999999999</v>
+      </c>
+      <c r="L17">
         <v>1.952</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>1.968</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>1.984</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>2</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>2.016</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>2.032</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>2.048</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>2.0640000000000001</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>2.08</v>
       </c>
-      <c r="T17">
-        <v>2.0960000000000001</v>
-      </c>
       <c r="U17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="V17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="W17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="X17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="Y17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="Z17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="AA17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="AB17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="AC17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="AD17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="AE17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
       <c r="AF17">
-        <v>2.0960000000000001</v>
+        <v>2.08</v>
       </c>
     </row>
   </sheetData>
@@ -9656,7 +9662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F4A00D-FEE1-4109-9021-DF78FFA4A8D5}">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AF49"/>
     </sheetView>
   </sheetViews>
@@ -9771,7 +9777,7 @@
         <v>3854.4</v>
       </c>
       <c r="C2">
-        <v>3854.4</v>
+        <v>4084.67</v>
       </c>
       <c r="D2">
         <v>3854.4</v>
@@ -9967,7 +9973,7 @@
         <v>4239.84</v>
       </c>
       <c r="C4">
-        <v>4239.84</v>
+        <v>4493.1400000000003</v>
       </c>
       <c r="D4">
         <v>4239.84</v>
@@ -10947,94 +10953,94 @@
         <v>3047.38</v>
       </c>
       <c r="C14">
-        <v>3038.14</v>
+        <v>3038.13</v>
       </c>
       <c r="D14">
-        <v>3029.17</v>
+        <v>3029.15</v>
       </c>
       <c r="E14">
-        <v>3025.37</v>
+        <v>3025.35</v>
       </c>
       <c r="F14">
-        <v>3023.83</v>
+        <v>3023.79</v>
       </c>
       <c r="G14">
-        <v>3022.98</v>
+        <v>3023.69</v>
       </c>
       <c r="H14">
-        <v>3012.73</v>
+        <v>3018.59</v>
       </c>
       <c r="I14">
-        <v>3008.33</v>
+        <v>3016.36</v>
       </c>
       <c r="J14">
-        <v>3008.2</v>
+        <v>3017.38</v>
       </c>
       <c r="K14">
-        <v>3003.77</v>
+        <v>3011.77</v>
       </c>
       <c r="L14">
-        <v>3003.41</v>
+        <v>3012.27</v>
       </c>
       <c r="M14">
-        <v>3004.03</v>
+        <v>3013.78</v>
       </c>
       <c r="N14">
-        <v>3006.23</v>
+        <v>3016.18</v>
       </c>
       <c r="O14">
-        <v>3006.54</v>
+        <v>3016.36</v>
       </c>
       <c r="P14">
-        <v>3003.68</v>
+        <v>3013.05</v>
       </c>
       <c r="Q14">
-        <v>3003.86</v>
+        <v>3013.59</v>
       </c>
       <c r="R14">
-        <v>3003.9</v>
+        <v>3013.18</v>
       </c>
       <c r="S14">
-        <v>3004.28</v>
+        <v>3013.73</v>
       </c>
       <c r="T14">
-        <v>3004.08</v>
+        <v>3014.1</v>
       </c>
       <c r="U14">
-        <v>3004.64</v>
+        <v>3014.82</v>
       </c>
       <c r="V14">
-        <v>3005.13</v>
+        <v>3015.36</v>
       </c>
       <c r="W14">
-        <v>3005.81</v>
+        <v>3016.2</v>
       </c>
       <c r="X14">
-        <v>3006.22</v>
+        <v>3016.67</v>
       </c>
       <c r="Y14">
-        <v>3007.22</v>
+        <v>3017.77</v>
       </c>
       <c r="Z14">
-        <v>3007.59</v>
+        <v>3018.27</v>
       </c>
       <c r="AA14">
-        <v>3008.38</v>
+        <v>3019</v>
       </c>
       <c r="AB14">
-        <v>3008.75</v>
+        <v>3019.38</v>
       </c>
       <c r="AC14">
-        <v>3009.25</v>
+        <v>3019.73</v>
       </c>
       <c r="AD14">
-        <v>3010.01</v>
+        <v>3020.39</v>
       </c>
       <c r="AE14">
-        <v>3010.88</v>
+        <v>3021.57</v>
       </c>
       <c r="AF14">
-        <v>3011.59</v>
+        <v>3022.18</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.35">
@@ -11140,97 +11146,97 @@
         <v>291</v>
       </c>
       <c r="B16">
-        <v>3461.76</v>
+        <v>3461.75</v>
       </c>
       <c r="C16">
-        <v>3477.08</v>
+        <v>3477.07</v>
       </c>
       <c r="D16">
-        <v>3492.55</v>
+        <v>3492.53</v>
       </c>
       <c r="E16">
-        <v>3513.89</v>
+        <v>3513.86</v>
       </c>
       <c r="F16">
-        <v>3537.79</v>
+        <v>3537.75</v>
       </c>
       <c r="G16">
-        <v>3553.93</v>
+        <v>3554.77</v>
       </c>
       <c r="H16">
-        <v>3567.48</v>
+        <v>3574.43</v>
       </c>
       <c r="I16">
-        <v>3587.84</v>
+        <v>3597.41</v>
       </c>
       <c r="J16">
-        <v>3613.25</v>
+        <v>3624.28</v>
       </c>
       <c r="K16">
-        <v>3633.45</v>
+        <v>3643.13</v>
       </c>
       <c r="L16">
-        <v>3658.55</v>
+        <v>3669.34</v>
       </c>
       <c r="M16">
-        <v>3667.8</v>
+        <v>3679.72</v>
       </c>
       <c r="N16">
-        <v>3670.5</v>
+        <v>3682.64</v>
       </c>
       <c r="O16">
-        <v>3679.4</v>
+        <v>3691.41</v>
       </c>
       <c r="P16">
-        <v>3684.41</v>
+        <v>3695.9</v>
       </c>
       <c r="Q16">
-        <v>3693.13</v>
+        <v>3705.09</v>
       </c>
       <c r="R16">
-        <v>3693.18</v>
+        <v>3704.59</v>
       </c>
       <c r="S16">
-        <v>3702.15</v>
+        <v>3713.81</v>
       </c>
       <c r="T16">
-        <v>3710.42</v>
+        <v>3722.79</v>
       </c>
       <c r="U16">
-        <v>3719.62</v>
+        <v>3732.23</v>
       </c>
       <c r="V16">
-        <v>3720.23</v>
+        <v>3732.89</v>
       </c>
       <c r="W16">
-        <v>3729.59</v>
+        <v>3742.47</v>
       </c>
       <c r="X16">
-        <v>3738.61</v>
+        <v>3751.61</v>
       </c>
       <c r="Y16">
-        <v>3748.38</v>
+        <v>3761.53</v>
       </c>
       <c r="Z16">
-        <v>3748.84</v>
+        <v>3762.15</v>
       </c>
       <c r="AA16">
-        <v>3758.35</v>
+        <v>3771.61</v>
       </c>
       <c r="AB16">
-        <v>3767.33</v>
+        <v>3780.64</v>
       </c>
       <c r="AC16">
-        <v>3776.49</v>
+        <v>3789.64</v>
       </c>
       <c r="AD16">
-        <v>3777.43</v>
+        <v>3790.47</v>
       </c>
       <c r="AE16">
-        <v>3787.06</v>
+        <v>3800.5</v>
       </c>
       <c r="AF16">
-        <v>3796.48</v>
+        <v>3809.83</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.35">
@@ -11241,94 +11247,94 @@
         <v>2103.9299999999998</v>
       </c>
       <c r="C17">
-        <v>2097.9</v>
+        <v>2097.92</v>
       </c>
       <c r="D17">
-        <v>2089.8000000000002</v>
+        <v>2089.9299999999998</v>
       </c>
       <c r="E17">
-        <v>2078.46</v>
+        <v>2078.75</v>
       </c>
       <c r="F17">
-        <v>2068.66</v>
+        <v>2069.08</v>
       </c>
       <c r="G17">
-        <v>2064.5100000000002</v>
+        <v>2065.63</v>
       </c>
       <c r="H17">
-        <v>2052.2399999999998</v>
+        <v>2059.5100000000002</v>
       </c>
       <c r="I17">
-        <v>2046.65</v>
+        <v>2056.11</v>
       </c>
       <c r="J17">
-        <v>2043.81</v>
+        <v>2054.67</v>
       </c>
       <c r="K17">
-        <v>2035.6</v>
+        <v>2045.67</v>
       </c>
       <c r="L17">
-        <v>2031.26</v>
+        <v>2043.08</v>
       </c>
       <c r="M17">
-        <v>2028.22</v>
+        <v>2041.87</v>
       </c>
       <c r="N17">
-        <v>2027.46</v>
+        <v>2042.02</v>
       </c>
       <c r="O17">
-        <v>2024.2</v>
+        <v>2039.38</v>
       </c>
       <c r="P17">
-        <v>2016.27</v>
+        <v>2031.62</v>
       </c>
       <c r="Q17">
-        <v>2012.54</v>
+        <v>2029.24</v>
       </c>
       <c r="R17">
-        <v>2008.6</v>
+        <v>2025.52</v>
       </c>
       <c r="S17">
-        <v>2005.26</v>
+        <v>2023.19</v>
       </c>
       <c r="T17">
-        <v>2001</v>
+        <v>2020.76</v>
       </c>
       <c r="U17">
-        <v>1998</v>
+        <v>2018.82</v>
       </c>
       <c r="V17">
-        <v>1995.15</v>
+        <v>2016.77</v>
       </c>
       <c r="W17">
-        <v>1992.54</v>
+        <v>2015.05</v>
       </c>
       <c r="X17">
-        <v>1989.49</v>
+        <v>2012.83</v>
       </c>
       <c r="Y17">
-        <v>1987.45</v>
+        <v>2011.6</v>
       </c>
       <c r="Z17">
-        <v>1984.54</v>
+        <v>2009.56</v>
       </c>
       <c r="AA17">
-        <v>1982.31</v>
+        <v>2007.92</v>
       </c>
       <c r="AB17">
-        <v>1979.13</v>
+        <v>2005.57</v>
       </c>
       <c r="AC17">
-        <v>1976.49</v>
+        <v>2003.29</v>
       </c>
       <c r="AD17">
-        <v>1974.27</v>
+        <v>2001.6</v>
       </c>
       <c r="AE17">
-        <v>1972.28</v>
+        <v>2000.89</v>
       </c>
       <c r="AF17">
-        <v>1970.1</v>
+        <v>1999.24</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.35">
@@ -11437,94 +11443,94 @@
         <v>2112.63</v>
       </c>
       <c r="C19">
-        <v>2123.91</v>
+        <v>2123.9299999999998</v>
       </c>
       <c r="D19">
-        <v>2132.98</v>
+        <v>2133.11</v>
       </c>
       <c r="E19">
-        <v>2138.58</v>
+        <v>2138.87</v>
       </c>
       <c r="F19">
-        <v>2154.14</v>
+        <v>2154.58</v>
       </c>
       <c r="G19">
-        <v>2166.89</v>
+        <v>2168.06</v>
       </c>
       <c r="H19">
-        <v>2170.96</v>
+        <v>2178.66</v>
       </c>
       <c r="I19">
-        <v>2190.4299999999998</v>
+        <v>2200.54</v>
       </c>
       <c r="J19">
-        <v>2204.27</v>
+        <v>2215.98</v>
       </c>
       <c r="K19">
-        <v>2212.2399999999998</v>
+        <v>2223.1799999999998</v>
       </c>
       <c r="L19">
-        <v>2232.71</v>
+        <v>2245.6999999999998</v>
       </c>
       <c r="M19">
-        <v>2237.75</v>
+        <v>2252.81</v>
       </c>
       <c r="N19">
-        <v>2245.2800000000002</v>
+        <v>2261.41</v>
       </c>
       <c r="O19">
-        <v>2250.0500000000002</v>
+        <v>2266.92</v>
       </c>
       <c r="P19">
-        <v>2249.5500000000002</v>
+        <v>2266.69</v>
       </c>
       <c r="Q19">
-        <v>2253.71</v>
+        <v>2272.42</v>
       </c>
       <c r="R19">
-        <v>2257.6</v>
+        <v>2276.62</v>
       </c>
       <c r="S19">
-        <v>2262.13</v>
+        <v>2282.36</v>
       </c>
       <c r="T19">
-        <v>2265.59</v>
+        <v>2287.96</v>
       </c>
       <c r="U19">
-        <v>2270.46</v>
+        <v>2294.12</v>
       </c>
       <c r="V19">
-        <v>2275.46</v>
+        <v>2300.11</v>
       </c>
       <c r="W19">
-        <v>2280.71</v>
+        <v>2306.48</v>
       </c>
       <c r="X19">
-        <v>2285.4499999999998</v>
+        <v>2312.2600000000002</v>
       </c>
       <c r="Y19">
-        <v>2291.3200000000002</v>
+        <v>2319.16</v>
       </c>
       <c r="Z19">
-        <v>2296.17</v>
+        <v>2325.11</v>
       </c>
       <c r="AA19">
-        <v>2301.77</v>
+        <v>2331.5100000000002</v>
       </c>
       <c r="AB19">
-        <v>2306.2600000000002</v>
+        <v>2337.0700000000002</v>
       </c>
       <c r="AC19">
-        <v>2311.35</v>
+        <v>2342.69</v>
       </c>
       <c r="AD19">
-        <v>2316.91</v>
+        <v>2348.9899999999998</v>
       </c>
       <c r="AE19">
-        <v>2322.7199999999998</v>
+        <v>2356.42</v>
       </c>
       <c r="AF19">
-        <v>2328.29</v>
+        <v>2362.7399999999998</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.35">
@@ -13005,7 +13011,7 @@
         <v>6640.08</v>
       </c>
       <c r="C35">
-        <v>6640.08</v>
+        <v>7036.78</v>
       </c>
       <c r="D35">
         <v>6640.08</v>
@@ -13201,7 +13207,7 @@
         <v>7305.84</v>
       </c>
       <c r="C37">
-        <v>7305.84</v>
+        <v>7742.31</v>
       </c>
       <c r="D37">
         <v>7305.84</v>
@@ -14474,13 +14480,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2F2634-68D9-4A99-92F0-3688E66AA3CB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1">
@@ -14495,12 +14504,12 @@
         <v>325</v>
       </c>
       <c r="B2">
-        <f>'STEO 7d'!J9/(SUM(Capacity!B2*'Capacity Factors'!B2,Capacity!B13*'Capacity Factors'!B35))*1000</f>
-        <v>0.8940388967769245</v>
+        <f>'STEO 7d'!J9/(SUM(Capacity!B2*'Capacity Factors'!B2,Capacity!B13*'Capacity Factors'!B35))*1000*B5</f>
+        <v>0.82698597951865516</v>
       </c>
       <c r="C2">
         <f>'STEO 7d'!K9/(SUM(Capacity!C2*'Capacity Factors'!C2,Capacity!C13*'Capacity Factors'!C35))*1000</f>
-        <v>1.0597433184427261</v>
+        <v>1.0000010797726713</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -14508,12 +14517,28 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <f>B2</f>
-        <v>0.8940388967769245</v>
+        <f>'STEO 7d'!J9/(SUM(Capacity!B2*'Capacity Factors'!B2,Capacity!B13*'Capacity Factors'!B35))*1000*B6</f>
+        <v>0.71523111742153966</v>
       </c>
       <c r="C3">
         <f>C2</f>
-        <v>1.0597433184427261</v>
+        <v>1.0000010797726713</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B6">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -14672,11 +14697,11 @@
       </c>
       <c r="G2">
         <f>'2020 Calculations'!B2</f>
-        <v>0.8940388967769245</v>
+        <v>0.82698597951865516</v>
       </c>
       <c r="H2">
         <f>'2020 Calculations'!C2</f>
-        <v>1.0597433184427261</v>
+        <v>1.0000010797726713</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -16228,11 +16253,11 @@
       </c>
       <c r="G13">
         <f>'2020 Calculations'!B3</f>
-        <v>0.8940388967769245</v>
+        <v>0.71523111742153966</v>
       </c>
       <c r="H13">
         <f>'2020 Calculations'!C3</f>
-        <v>1.0597433184427261</v>
+        <v>1.0000010797726713</v>
       </c>
       <c r="I13">
         <v>0</v>

</xml_diff>

<commit_message>
Make BGDPbES Excel file match .csv file (using no guaranteed dispatch in BAU case) (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0533CB9-F848-4B7A-8C34-704F27035DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB1BF7A-AF18-46D6-AD11-ACCE60D44E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18615" yWindow="2085" windowWidth="29370" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13440" yWindow="1365" windowWidth="29370" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1088,7 +1088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1106,7 +1106,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -6340,7 +6339,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>289</v>
       </c>
       <c r="B1" t="s">
@@ -8180,15 +8179,15 @@
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23">
         <f>SUMIFS(C$2:C$18,$A$2:$A$18,$A23)/10^6</f>
         <v>1423.79367</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23">
         <f t="shared" ref="C23:D23" si="0">SUMIFS(D$2:D$18,$A$2:$A$18,$A23)/10^6</f>
         <v>1380.1169600000001</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <f t="shared" si="0"/>
         <v>1327.7883099999999</v>
       </c>
@@ -8197,15 +8196,15 @@
       <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24">
         <f t="shared" ref="B24:D35" si="1">SUMIFS(C$2:C$18,$A$2:$A$18,$A24)/10^6</f>
         <v>893.91160000000002</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24">
         <f t="shared" si="1"/>
         <v>935.76189999999997</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24">
         <f t="shared" si="1"/>
         <v>893.20590000000004</v>
       </c>
@@ -8214,15 +8213,15 @@
       <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25">
         <f t="shared" si="1"/>
         <v>804.06299999999999</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25">
         <f t="shared" si="1"/>
         <v>804.06299999999999</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25">
         <f t="shared" si="1"/>
         <v>808.22400000000005</v>
       </c>
@@ -8231,15 +8230,15 @@
       <c r="A26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8248,15 +8247,15 @@
       <c r="A27" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27">
         <f t="shared" si="1"/>
         <v>282.77999999999997</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27">
         <f t="shared" si="1"/>
         <v>283.12799999999999</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27">
         <f t="shared" si="1"/>
         <v>283.18400000000003</v>
       </c>
@@ -8265,15 +8264,15 @@
       <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28">
         <f t="shared" si="1"/>
         <v>401.88924600000001</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28">
         <f t="shared" si="1"/>
         <v>458.27236499999998</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <f t="shared" si="1"/>
         <v>488.39535100000001</v>
       </c>
@@ -8282,15 +8281,15 @@
       <c r="A29" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29">
         <f t="shared" si="1"/>
         <v>124.22653</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29">
         <f t="shared" si="1"/>
         <v>172.06853000000001</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29">
         <f t="shared" si="1"/>
         <v>230.50153</v>
       </c>
@@ -8299,15 +8298,15 @@
       <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30">
         <f t="shared" si="1"/>
         <v>3.3512</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30">
         <f t="shared" si="1"/>
         <v>22.730399999999999</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30">
         <f t="shared" si="1"/>
         <v>42.8992</v>
       </c>
@@ -8316,15 +8315,15 @@
       <c r="A31" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31">
         <f t="shared" si="1"/>
         <v>9.3732000000000006</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31">
         <f t="shared" si="1"/>
         <v>9.5554100000000002</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31">
         <f t="shared" si="1"/>
         <v>9.7376199999999997</v>
       </c>
@@ -8333,15 +8332,15 @@
       <c r="A32" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8350,15 +8349,15 @@
       <c r="A33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8367,15 +8366,15 @@
       <c r="A34" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8384,15 +8383,15 @@
       <c r="A35" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35">
         <f t="shared" si="1"/>
         <v>15.4153</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35">
         <f t="shared" si="1"/>
         <v>15.415800000000001</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35">
         <f t="shared" si="1"/>
         <v>15.415800000000001</v>
       </c>
@@ -10179,7 +10178,7 @@
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>308</v>
       </c>
     </row>
@@ -11964,7 +11963,7 @@
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>326</v>
       </c>
     </row>
@@ -14286,11 +14285,11 @@
       </c>
       <c r="B2">
         <f>'STEO 7d'!J$9/(SUM(Capacity!B$2/1000*'Capacity Factors'!B$22,Capacity!B$14/1000*'Capacity Factors'!B$34))*1000*B5</f>
-        <v>0.80449728253770403</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>'STEO 7d'!K$9/(SUM(Capacity!C$2/1000*'Capacity Factors'!C$22,Capacity!C$14/1000*'Capacity Factors'!C$34))*1000*C5</f>
-        <v>0.95401995059599998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -14299,11 +14298,11 @@
       </c>
       <c r="B3">
         <f>'STEO 7d'!J$9/(SUM(Capacity!B$2/1000*'Capacity Factors'!B$22,Capacity!B$14/1000*'Capacity Factors'!B$34))*1000*B6</f>
-        <v>0.80449728253770403</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>'STEO 7d'!K$9/(SUM(Capacity!C$2/1000*'Capacity Factors'!C$22,Capacity!C$14/1000*'Capacity Factors'!C$34))*1000*C6</f>
-        <v>0.95401995059599998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -14311,10 +14310,10 @@
         <v>268</v>
       </c>
       <c r="B5" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -14322,10 +14321,10 @@
         <v>268</v>
       </c>
       <c r="B6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14482,11 +14481,11 @@
       </c>
       <c r="G2">
         <f>'2020 Calculations'!B2</f>
-        <v>0.80449728253770403</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f>'2020 Calculations'!C2</f>
-        <v>0.95401995059599998</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -16179,11 +16178,11 @@
       </c>
       <c r="G14">
         <f>'2020 Calculations'!B3</f>
-        <v>0.80449728253770403</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <f>'2020 Calculations'!C3</f>
-        <v>0.95401995059599998</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>0</v>

</xml_diff>

<commit_message>
Fix for Weibull curves, set nuclear to guaranteed dispatch, and new BAU retirements data to exclude AEO's economic retirements
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB1BF7A-AF18-46D6-AD11-ACCE60D44E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93718E2E-F7ED-46C1-AC90-A166D37C74FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="1365" windowWidth="29370" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1449,7 +1449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -14339,7 +14341,9 @@
   </sheetPr>
   <dimension ref="A1:AK18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14890,140 +14894,139 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -15760,11 +15763,9 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L11">

</xml_diff>

<commit_message>
Adds a check to see if positive cost resources are need for the RPS. This mostly helps avoid dispatching resources that qualify for the RPS when the RPS is turned off (like certain hydrogen plants). CCS plants are moved to guaranteed dispatch.
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C675A6B7-1944-4BEB-ADA5-F2D2872020CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB189523-7579-4160-B2F5-DB3ADF084D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -599,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2482,8 +2482,8 @@
   </sheetPr>
   <dimension ref="A1:AK25"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:AK25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,112 +4933,112 @@
         <v>53</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -5046,112 +5046,112 @@
         <v>54</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -5159,112 +5159,112 @@
         <v>55</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -5272,112 +5272,112 @@
         <v>56</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>